<commit_message>
feat: Introduce Excel data processing and beban calculation module along with new input data files.
</commit_message>
<xml_diff>
--- a/Rencana/RENCANA.xlsx
+++ b/Rencana/RENCANA.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\odooCompressionTest\Rencana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BB6FB-C65C-468B-AA64-8C9236063D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278EA9D5-A0D6-484B-815A-9883DA9237A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Excel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Report Excel'!$A$1:$V$88</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="123">
-  <si>
-    <t>2025-12-05</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="111">
+  <si>
+    <t>2025-12-24</t>
   </si>
   <si>
     <t>Docket</t>
@@ -94,64 +91,220 @@
     <t>Persentase Kekuatan (%)</t>
   </si>
   <si>
-    <t>DOCKET/PTB/11-2025/25282</t>
+    <t>DOCKET/PTB/11-2025/26332</t>
+  </si>
+  <si>
+    <t>SO/DIR2/DV2-4/11-2025/3281</t>
+  </si>
+  <si>
+    <t>SPP/PTB/11-2025/1706</t>
+  </si>
+  <si>
+    <t>Pembangunan Jalan Tol  Akses Patimban Paket 3</t>
+  </si>
+  <si>
+    <t>HUTAMA KARYA - JAYA KONSTRUKSI JOINT OPERATION</t>
+  </si>
+  <si>
+    <t>Class B-2 FA</t>
+  </si>
+  <si>
+    <t>Silinder 15 x 30 cm</t>
+  </si>
+  <si>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / BP P2 - 16 JEMBATAN PERTAGAS STA 31+547 / CLASS B-2 SCC / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26335</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26362</t>
   </si>
   <si>
     <t>SO/DIR2/DV2-4/11-2025/3282</t>
   </si>
   <si>
-    <t>SPP/PTB/11-2025/1681</t>
-  </si>
-  <si>
-    <t>Pembangunan Jalan Tol  Akses Patimban Paket 3</t>
-  </si>
-  <si>
-    <t>HUTAMA KARYA - JAYA KONSTRUKSI JOINT OPERATION</t>
+    <t>SPP/PTB/11-2025/1704</t>
+  </si>
+  <si>
+    <t>Class E-1 FA</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / LC P2 BRIDGE 20 / CLASS E / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26308</t>
   </si>
   <si>
     <t>Class B-1 FA</t>
   </si>
   <si>
-    <t>Silinder 15 x 30 cm</t>
-  </si>
-  <si>
-    <t>Tidak</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / PILEHEAD GRID A4 A5 A6 A7 A8 A11 A12 PS 16 STA 32+550 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25284</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25286</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25297</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25311</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / WALL ABUTMENT A2 STG 2 OP 6 STA 32+048 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25315</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25309</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / WINGWALL BC STA 33+214 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25303</t>
+    <t>HK - JAKON JO / PILEHEAD A31 B32 PS16 STA 31+750 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26312</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26303</t>
+  </si>
+  <si>
+    <t>SO/DIR2/DV2-4/11-2025/3283</t>
+  </si>
+  <si>
+    <t>SPP/PTB/11-2025/1715</t>
+  </si>
+  <si>
+    <t>Patimban Access Toll Road P02 (JOI 60%)</t>
+  </si>
+  <si>
+    <t>WASKITA - ABIPRAYA JO</t>
+  </si>
+  <si>
+    <t>Class E-1 NFA</t>
+  </si>
+  <si>
+    <t>WASKITA - ABP JO / LC AKSES WARGA SENGON KE STA 27 / CLASS E / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26305</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26340</t>
+  </si>
+  <si>
+    <t>SO/DIR2/DV2-4/11-2025/3286</t>
+  </si>
+  <si>
+    <t>SPP/PTB/11-2025/1705</t>
+  </si>
+  <si>
+    <t>JALAN TOL AKSES PATIMBAN PAKET 4</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO</t>
+  </si>
+  <si>
+    <t>Class B-1 NFA</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / KOLOM STG 1 P3W MB 25 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26353</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26316</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / PARAPET A1-A2E MB 24 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26319</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26306</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / PARAPET SPAN 5 &amp; 6 OUTER IC 02 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26310</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26326</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / PIERHEAD STG 1 P4E MB 25 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26329</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26354</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB P10 - P11W MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26361</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26370</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26317</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB P7 - P8W MB22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26322</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26341</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26350</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB W4E - WEJ4 PS 17 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26364</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/11-2025/26372</t>
+  </si>
+  <si>
+    <t>SO/DIR2/DV2-4/11-2025/3397</t>
+  </si>
+  <si>
+    <t>SPP/PTB/11-2025/1722</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27640</t>
+  </si>
+  <si>
+    <t>SO/DIR2/DV2-4/12-2025/3469</t>
+  </si>
+  <si>
+    <t>SPP/PTB/12-2025/1763</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / HALFSLAB S1' (8 UNIT), S1AD' (1 UNIT) PS 14 STA 31+100 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27687</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / TOP SLAB A97 - AW1 PS 14 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27641</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / TOP SLAB PW1 - PW2 BRIDGE 17 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27645</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27650</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27665</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27636</t>
   </si>
   <si>
     <t>SO/DIR2/DV2-4/10-2025/3259</t>
   </si>
   <si>
-    <t>SPP/PTB/11-2025/1676</t>
+    <t>SPP/PTB/12-2025/1765</t>
   </si>
   <si>
     <t>JALAN TOL AKSES PATIMBAN</t>
@@ -163,235 +316,43 @@
     <t>Fc-30 NFA</t>
   </si>
   <si>
-    <t>PP - TOL PTB / MEDIAN CONCRETE BARIER STA 16+900 / FC 30 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25287</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3283</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1685</t>
-  </si>
-  <si>
-    <t>Patimban Access Toll Road P02 (JOI 60%)</t>
-  </si>
-  <si>
-    <t>WASKITA - ABIPRAYA JO</t>
-  </si>
-  <si>
-    <t>Class C-1 NFA</t>
-  </si>
-  <si>
-    <t>WASKITA - ABP JO / AKSES DETOUR KRANJAT / CLASS C-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25281</t>
-  </si>
-  <si>
-    <t>Class B-1 NFA</t>
-  </si>
-  <si>
-    <t>WASKITA - ABP JO / PH W.8.7A &amp; E.8.7A (PS 8) STA 26+200 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25289</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3286</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1682</t>
-  </si>
-  <si>
-    <t>JALAN TOL AKSES PATIMBAN PAKET 4</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PIERHEAD P15 MB 22 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25291</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25299</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PILEHEAD PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25302</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25313</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / STUFFING PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/25314</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26487</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3281</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1717</t>
-  </si>
-  <si>
-    <t>Class B-2 FA</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / BP P2 - 14 JEMBATAN PERTAGAS STA 31+547 / CLASS B-2 SCC / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26491</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26472</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3381</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1714</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / WALL ABT A2 STG 4 OP 6 STA 32+048 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26485</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26444</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3371</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1710</t>
-  </si>
-  <si>
-    <t>Proyek Pekerjaan Fasilitas Workshop PGT Patimban</t>
-  </si>
-  <si>
-    <t>PT. SAMUDERA REKSO ASRI</t>
-  </si>
-  <si>
-    <t>K-350 NFA</t>
-  </si>
-  <si>
-    <t>PT SRA / K 350 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26498</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3429</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1724</t>
-  </si>
-  <si>
-    <t>Pekerjaan Siphon Sisi Timur Bendung Salamdarma</t>
-  </si>
-  <si>
-    <t>PT. NINDYA KARYA</t>
-  </si>
-  <si>
-    <t>K-300 NFA</t>
-  </si>
-  <si>
-    <t>PT. NINDYA KARYA / K 300 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26506</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26508</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26469</t>
-  </si>
-  <si>
-    <t>K-175 NFA</t>
-  </si>
-  <si>
-    <t>PT. NINDYA KARYA / LC / K 175 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26460</t>
-  </si>
-  <si>
-    <t>SO/DIR2/DV2-4/11-2025/3397</t>
-  </si>
-  <si>
-    <t>SPP/PTB/11-2025/1722</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / DECKSLAB RAMP 8 IC 06 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26464</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26470</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26441</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / DECKSLAB SPAN 3W IC 02 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26448</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26456</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26452</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / DIAFRAGMA P1 - A2W MB23 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26453</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26475</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PILEHEAD W8E - W8I PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26483</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26457</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PILEHEAD WEJ6 PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26459</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26494</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PILESLAB WEJ4 - W5E PS17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26499</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/11-2025/26503</t>
+    <t>PP - TOL PTB / RC SLAB PW 29 - ABT 1 B8 / FC 30 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27662</t>
+  </si>
+  <si>
+    <t>SPP/PTB/12-2025/1766</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / FOOTING A2W MB 21 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27669</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27678</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27654</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / RC SLAB P15 - P14E MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27667</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27679</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27637</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / WALL + TOP SLAB BOX CULVERT RAMP 4 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/27639</t>
   </si>
 </sst>
 </file>
@@ -766,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V81"/>
+  <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,13 +979,13 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -1033,7 +994,7 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -1054,18 +1015,18 @@
         <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -1074,7 +1035,7 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -1095,18 +1056,18 @@
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -1115,7 +1076,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1136,18 +1097,18 @@
         <v>30</v>
       </c>
       <c r="P8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -1156,7 +1117,7 @@
         <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1177,27 +1138,27 @@
         <v>30</v>
       </c>
       <c r="P9" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -1218,27 +1179,27 @@
         <v>30</v>
       </c>
       <c r="P10" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G11">
         <v>4</v>
@@ -1259,27 +1220,27 @@
         <v>30</v>
       </c>
       <c r="P11" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1300,27 +1261,27 @@
         <v>30</v>
       </c>
       <c r="P12" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -1341,27 +1302,27 @@
         <v>30</v>
       </c>
       <c r="P13" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G14">
         <v>3</v>
@@ -1382,27 +1343,27 @@
         <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -1423,24 +1384,24 @@
         <v>30</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
@@ -1464,24 +1425,24 @@
         <v>30</v>
       </c>
       <c r="P16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
         <v>55</v>
@@ -1505,24 +1466,24 @@
         <v>30</v>
       </c>
       <c r="P17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
         <v>55</v>
@@ -1551,19 +1512,19 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -1595,16 +1556,16 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
         <v>55</v>
@@ -1636,16 +1597,16 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
         <v>55</v>
@@ -1677,16 +1638,16 @@
         <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
         <v>55</v>
@@ -1718,16 +1679,16 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
         <v>55</v>
@@ -1759,16 +1720,16 @@
         <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
         <v>55</v>
@@ -1800,16 +1761,16 @@
         <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
         <v>55</v>
@@ -1841,16 +1802,16 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
         <v>55</v>
@@ -1882,16 +1843,16 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F27" t="s">
         <v>55</v>
@@ -1923,16 +1884,16 @@
         <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -1964,16 +1925,16 @@
         <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F29" t="s">
         <v>55</v>
@@ -2002,22 +1963,22 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G30">
         <v>3</v>
@@ -2038,27 +1999,27 @@
         <v>30</v>
       </c>
       <c r="P30" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G31">
         <v>4</v>
@@ -2079,27 +2040,27 @@
         <v>30</v>
       </c>
       <c r="P31" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G32">
         <v>3</v>
@@ -2120,27 +2081,27 @@
         <v>30</v>
       </c>
       <c r="P32" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G33">
         <v>4</v>
@@ -2161,683 +2122,683 @@
         <v>30</v>
       </c>
       <c r="P33" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J34" t="s">
         <v>29</v>
       </c>
       <c r="K34">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O34" t="s">
         <v>30</v>
       </c>
       <c r="P34" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H35" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J35" t="s">
         <v>29</v>
       </c>
       <c r="K35">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O35" t="s">
         <v>30</v>
       </c>
       <c r="P35" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H36" t="s">
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J36" t="s">
         <v>29</v>
       </c>
       <c r="K36">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O36" t="s">
         <v>30</v>
       </c>
       <c r="P36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H37" t="s">
         <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J37" t="s">
         <v>29</v>
       </c>
       <c r="K37">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O37" t="s">
         <v>30</v>
       </c>
       <c r="P37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
         <v>55</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H38" t="s">
         <v>0</v>
       </c>
       <c r="I38" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J38" t="s">
         <v>29</v>
       </c>
       <c r="K38">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O38" t="s">
         <v>30</v>
       </c>
       <c r="P38" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
         <v>55</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H39" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J39" t="s">
         <v>29</v>
       </c>
       <c r="K39">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O39" t="s">
         <v>30</v>
       </c>
       <c r="P39" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
         <v>55</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H40" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J40" t="s">
         <v>29</v>
       </c>
       <c r="K40">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O40" t="s">
         <v>30</v>
       </c>
       <c r="P40" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
         <v>55</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H41" t="s">
         <v>0</v>
       </c>
       <c r="I41" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J41" t="s">
         <v>29</v>
       </c>
       <c r="K41">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O41" t="s">
         <v>30</v>
       </c>
       <c r="P41" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
         <v>55</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H42" t="s">
         <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J42" t="s">
         <v>29</v>
       </c>
       <c r="K42">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O42" t="s">
         <v>30</v>
       </c>
       <c r="P42" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F43" t="s">
         <v>55</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H43" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J43" t="s">
         <v>29</v>
       </c>
       <c r="K43">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O43" t="s">
         <v>30</v>
       </c>
       <c r="P43" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F44" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H44" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J44" t="s">
         <v>29</v>
       </c>
       <c r="K44">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O44" t="s">
         <v>30</v>
       </c>
       <c r="P44" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H45" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J45" t="s">
         <v>29</v>
       </c>
       <c r="K45">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O45" t="s">
         <v>30</v>
       </c>
       <c r="P45" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H46" t="s">
         <v>0</v>
       </c>
       <c r="I46" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J46" t="s">
         <v>29</v>
       </c>
       <c r="K46">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O46" t="s">
         <v>30</v>
       </c>
       <c r="P46" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H47" t="s">
         <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J47" t="s">
         <v>29</v>
       </c>
       <c r="K47">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O47" t="s">
         <v>30</v>
       </c>
       <c r="P47" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="D48" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H48" t="s">
         <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J48" t="s">
         <v>29</v>
       </c>
       <c r="K48">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O48" t="s">
         <v>30</v>
       </c>
       <c r="P48" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H49" t="s">
         <v>0</v>
       </c>
       <c r="I49" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J49" t="s">
         <v>29</v>
       </c>
       <c r="K49">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O49" t="s">
         <v>30</v>
       </c>
       <c r="P49" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2858,27 +2819,27 @@
         <v>30</v>
       </c>
       <c r="P50" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E51" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G51">
         <v>2</v>
@@ -2899,27 +2860,27 @@
         <v>30</v>
       </c>
       <c r="P51" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2940,27 +2901,27 @@
         <v>30</v>
       </c>
       <c r="P52" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G53">
         <v>2</v>
@@ -2981,27 +2942,27 @@
         <v>30</v>
       </c>
       <c r="P53" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3022,27 +2983,27 @@
         <v>30</v>
       </c>
       <c r="P54" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G55">
         <v>2</v>
@@ -3063,27 +3024,27 @@
         <v>30</v>
       </c>
       <c r="P55" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E56" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3104,27 +3065,27 @@
         <v>30</v>
       </c>
       <c r="P56" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E57" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -3145,27 +3106,27 @@
         <v>30</v>
       </c>
       <c r="P57" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F58" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -3186,27 +3147,27 @@
         <v>30</v>
       </c>
       <c r="P58" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D59" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G59">
         <v>2</v>
@@ -3227,27 +3188,27 @@
         <v>30</v>
       </c>
       <c r="P59" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F60" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -3268,27 +3229,27 @@
         <v>30</v>
       </c>
       <c r="P60" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F61" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G61">
         <v>2</v>
@@ -3309,27 +3270,27 @@
         <v>30</v>
       </c>
       <c r="P61" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="F62" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -3350,27 +3311,27 @@
         <v>30</v>
       </c>
       <c r="P62" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D63" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="F63" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -3391,24 +3352,24 @@
         <v>30</v>
       </c>
       <c r="P63" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -3432,24 +3393,24 @@
         <v>30</v>
       </c>
       <c r="P64" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3473,24 +3434,24 @@
         <v>30</v>
       </c>
       <c r="P65" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F66" t="s">
         <v>55</v>
@@ -3514,24 +3475,24 @@
         <v>30</v>
       </c>
       <c r="P66" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F67" t="s">
         <v>55</v>
@@ -3555,27 +3516,27 @@
         <v>30</v>
       </c>
       <c r="P67" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F68" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -3596,27 +3557,27 @@
         <v>30</v>
       </c>
       <c r="P68" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="D69" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E69" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F69" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G69">
         <v>2</v>
@@ -3637,27 +3598,27 @@
         <v>30</v>
       </c>
       <c r="P69" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="D70" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E70" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F70" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -3678,27 +3639,27 @@
         <v>30</v>
       </c>
       <c r="P70" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="D71" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E71" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F71" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G71">
         <v>2</v>
@@ -3719,27 +3680,27 @@
         <v>30</v>
       </c>
       <c r="P71" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E72" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F72" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -3760,27 +3721,27 @@
         <v>30</v>
       </c>
       <c r="P72" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E73" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F73" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="G73">
         <v>2</v>
@@ -3801,27 +3762,27 @@
         <v>30</v>
       </c>
       <c r="P73" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C74" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D74" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E74" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F74" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -3842,27 +3803,27 @@
         <v>30</v>
       </c>
       <c r="P74" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D75" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F75" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G75">
         <v>2</v>
@@ -3883,27 +3844,27 @@
         <v>30</v>
       </c>
       <c r="P75" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E76" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F76" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -3924,27 +3885,27 @@
         <v>30</v>
       </c>
       <c r="P76" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D77" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E77" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G77">
         <v>2</v>
@@ -3965,27 +3926,27 @@
         <v>30</v>
       </c>
       <c r="P77" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D78" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E78" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F78" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -4006,27 +3967,27 @@
         <v>30</v>
       </c>
       <c r="P78" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D79" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E79" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F79" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="G79">
         <v>2</v>
@@ -4047,97 +4008,10 @@
         <v>30</v>
       </c>
       <c r="P79" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" t="s">
-        <v>82</v>
-      </c>
-      <c r="C80" t="s">
-        <v>83</v>
-      </c>
-      <c r="D80" t="s">
-        <v>84</v>
-      </c>
-      <c r="E80" t="s">
-        <v>85</v>
-      </c>
-      <c r="F80" t="s">
-        <v>86</v>
-      </c>
-      <c r="G80">
-        <v>1</v>
-      </c>
-      <c r="H80" t="s">
-        <v>0</v>
-      </c>
-      <c r="I80" s="2">
-        <v>7</v>
-      </c>
-      <c r="J80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K80">
-        <v>65</v>
-      </c>
-      <c r="O80" t="s">
-        <v>30</v>
-      </c>
-      <c r="P80" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" t="s">
-        <v>83</v>
-      </c>
-      <c r="D81" t="s">
-        <v>84</v>
-      </c>
-      <c r="E81" t="s">
-        <v>85</v>
-      </c>
-      <c r="F81" t="s">
-        <v>86</v>
-      </c>
-      <c r="G81">
-        <v>2</v>
-      </c>
-      <c r="H81" t="s">
-        <v>0</v>
-      </c>
-      <c r="I81" s="2">
-        <v>7</v>
-      </c>
-      <c r="J81" t="s">
-        <v>29</v>
-      </c>
-      <c r="K81">
-        <v>65</v>
-      </c>
-      <c r="O81" t="s">
-        <v>30</v>
-      </c>
-      <c r="P81" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V88" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V82">
-      <sortCondition descending="1" ref="I1:I88"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>